<commit_message>
refix: seperate money type for branch revenue
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9582FC-883B-4110-AF60-CE2C3156112C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9597C770-297A-427B-9FB3-C38F12145307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>BÁO CÁO DOANH THU</t>
   </si>
@@ -56,18 +56,12 @@
     <t>Chi nhánh</t>
   </si>
   <si>
-    <t>Tổng hàng</t>
-  </si>
-  <si>
     <t>Tổng khuyến mãi</t>
   </si>
   <si>
     <t>Tổng giảm giá</t>
   </si>
   <si>
-    <t>Doanh thu</t>
-  </si>
-  <si>
     <t>Tổng xu</t>
   </si>
   <si>
@@ -78,6 +72,21 @@
   </si>
   <si>
     <t>Tổng đơn hàng</t>
+  </si>
+  <si>
+    <t>Tổng tiền hàng</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng doanh thu tiền mặt </t>
+  </si>
+  <si>
+    <t>Tổng doanh thu chuyển khoản ngân hàng</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu ví nội bộ</t>
   </si>
 </sst>
 </file>
@@ -157,14 +166,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,72 +509,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DBBB0D-6011-49B5-900C-FA0A48448A03}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="19.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="19.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" ht="43.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -573,32 +588,41 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>9</v>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>